<commit_message>
created appl stock yearly earnings per share bar chart
</commit_message>
<xml_diff>
--- a/aapl_stock_yearly_earnings_per_share_df.xlsx
+++ b/aapl_stock_yearly_earnings_per_share_df.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27231"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/25ac2033dcfcea55/Desktop/ALIENWARE - 2023-04_24 - Onwards/Python/Stock Market Data/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_C1C5873A2630921FD2FE31D2F8F2D3C2D4599232" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2C8046CB-7B34-4596-8F35-C0623CAE50CC}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -67,8 +61,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -131,21 +125,13 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -183,7 +169,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -217,7 +203,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -252,10 +237,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -428,25 +412,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:E5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -469,7 +442,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" s="1">
         <v>8</v>
       </c>
@@ -486,7 +459,7 @@
         <v>40.03</v>
       </c>
       <c r="F2">
-        <v>925231076.69200003</v>
+        <v>925231076.692</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
@@ -495,7 +468,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3" s="1">
         <v>9</v>
       </c>
@@ -512,7 +485,7 @@
         <v>6.49</v>
       </c>
       <c r="F3">
-        <v>6087827426.8100004</v>
+        <v>6087827426.81</v>
       </c>
       <c r="G3" t="s">
         <v>12</v>
@@ -521,7 +494,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4" s="1">
         <v>10</v>
       </c>
@@ -535,10 +508,10 @@
         <v>10</v>
       </c>
       <c r="E4">
-        <v>9.2799999999999994</v>
+        <v>9.279999999999999</v>
       </c>
       <c r="F4">
-        <v>5753663793.1000004</v>
+        <v>5753663793.1</v>
       </c>
       <c r="G4" t="s">
         <v>12</v>
@@ -547,7 +520,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5" s="1">
         <v>11</v>
       </c>
@@ -564,7 +537,7 @@
         <v>8.35</v>
       </c>
       <c r="F5">
-        <v>5471497005.9899998</v>
+        <v>5471497005.99</v>
       </c>
       <c r="G5" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
correction - created appl stock yearly earnings per share pie chart
</commit_message>
<xml_diff>
--- a/aapl_stock_yearly_earnings_per_share_df.xlsx
+++ b/aapl_stock_yearly_earnings_per_share_df.xlsx
@@ -413,136 +413,124 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:7">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="1">
+    <row r="2" spans="1:7">
+      <c r="A2">
         <v>8</v>
       </c>
-      <c r="B2">
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2">
+        <v>40.03</v>
+      </c>
+      <c r="E2">
+        <v>925231076.692</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2">
-        <v>40.03</v>
-      </c>
-      <c r="F2">
-        <v>925231076.692</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3">
+        <v>6.49</v>
+      </c>
+      <c r="E3">
+        <v>6087827426.81</v>
+      </c>
+      <c r="F3" t="s">
         <v>12</v>
       </c>
-      <c r="H2" t="s">
+      <c r="G3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="1">
-        <v>9</v>
-      </c>
-      <c r="B3">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
+    <row r="4" spans="1:7">
+      <c r="A4">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
         <v>7</v>
       </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3">
-        <v>6.49</v>
-      </c>
-      <c r="F3">
-        <v>6087827426.81</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4">
+        <v>9.279999999999999</v>
+      </c>
+      <c r="E4">
+        <v>5753663793.1</v>
+      </c>
+      <c r="F4" t="s">
         <v>12</v>
       </c>
-      <c r="H3" t="s">
+      <c r="G4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="1">
-        <v>10</v>
-      </c>
-      <c r="B4">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
+    <row r="5" spans="1:7">
+      <c r="A5">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
         <v>7</v>
       </c>
-      <c r="D4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4">
-        <v>9.279999999999999</v>
-      </c>
-      <c r="F4">
-        <v>5753663793.1</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5">
+        <v>8.35</v>
+      </c>
+      <c r="E5">
+        <v>5471497005.99</v>
+      </c>
+      <c r="F5" t="s">
         <v>12</v>
       </c>
-      <c r="H4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="1">
-        <v>11</v>
-      </c>
-      <c r="B5">
-        <v>11</v>
-      </c>
-      <c r="C5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5">
-        <v>8.35</v>
-      </c>
-      <c r="F5">
-        <v>5471497005.99</v>
-      </c>
       <c r="G5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H5" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
created msft stock yearly earnings per share dataframe
</commit_message>
<xml_diff>
--- a/aapl_stock_yearly_earnings_per_share_df.xlsx
+++ b/aapl_stock_yearly_earnings_per_share_df.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27231"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/25ac2033dcfcea55/Desktop/ALIENWARE - 2023-04_24 - Onwards/Python/Stock Market Data/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_6F58E73C2630921FD2FE31D2F8F2D3C224DA7512" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C94036C7-084C-477C-B109-A1A028131F2B}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -67,8 +61,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -131,21 +125,13 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -183,7 +169,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -217,7 +203,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -252,10 +237,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -428,25 +412,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -469,7 +442,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>8</v>
       </c>
@@ -483,7 +456,7 @@
         <v>40.03</v>
       </c>
       <c r="E2">
-        <v>925231076.69200003</v>
+        <v>925231076.692</v>
       </c>
       <c r="F2" t="s">
         <v>12</v>
@@ -492,7 +465,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>9</v>
       </c>
@@ -506,7 +479,7 @@
         <v>6.49</v>
       </c>
       <c r="E3">
-        <v>6087827426.8100004</v>
+        <v>6087827426.81</v>
       </c>
       <c r="F3" t="s">
         <v>12</v>
@@ -515,7 +488,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>10</v>
       </c>
@@ -526,10 +499,10 @@
         <v>10</v>
       </c>
       <c r="D4">
-        <v>9.2799999999999994</v>
+        <v>9.279999999999999</v>
       </c>
       <c r="E4">
-        <v>5753663793.1000004</v>
+        <v>5753663793.1</v>
       </c>
       <c r="F4" t="s">
         <v>12</v>
@@ -538,7 +511,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>11</v>
       </c>
@@ -552,7 +525,7 @@
         <v>8.35</v>
       </c>
       <c r="E5">
-        <v>5471497005.9899998</v>
+        <v>5471497005.99</v>
       </c>
       <c r="F5" t="s">
         <v>12</v>

</xml_diff>